<commit_message>
update testcase create edit delete service
</commit_message>
<xml_diff>
--- a/src/main/resources/excels/BuyLinkTCs.xlsx
+++ b/src/main/resources/excels/BuyLinkTCs.xlsx
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="77">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -308,12 +308,16 @@
   <si>
     <t>The buy link should not be shown in management page.
 Home page should be shown after navigated</t>
+  </si>
+  <si>
+    <t>PASS</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -679,10 +683,10 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="32.33203125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="65.6640625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="42" customWidth="1" collapsed="1"/>
-    <col min="5" max="5" width="18" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" customWidth="true" width="32.33203125" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="65.6640625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="18.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
@@ -715,6 +719,9 @@
       <c r="D2" s="4" t="s">
         <v>7</v>
       </c>
+      <c r="E2" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="3" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
@@ -827,6 +834,9 @@
       <c r="D10" s="4" t="s">
         <v>54</v>
       </c>
+      <c r="E10" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="11" spans="1:5" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
@@ -841,6 +851,9 @@
       <c r="D11" s="4" t="s">
         <v>55</v>
       </c>
+      <c r="E11" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="12" spans="1:5" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
@@ -855,6 +868,9 @@
       <c r="D12" s="4" t="s">
         <v>57</v>
       </c>
+      <c r="E12" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="13" spans="1:5" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
@@ -869,6 +885,9 @@
       <c r="D13" s="4" t="s">
         <v>59</v>
       </c>
+      <c r="E13" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="14" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
@@ -883,6 +902,9 @@
       <c r="D14" s="4" t="s">
         <v>61</v>
       </c>
+      <c r="E14" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="15" spans="1:5" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
@@ -897,6 +919,9 @@
       <c r="D15" s="4" t="s">
         <v>61</v>
       </c>
+      <c r="E15" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="16" spans="1:5" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
@@ -911,6 +936,9 @@
       <c r="D16" s="4" t="s">
         <v>64</v>
       </c>
+      <c r="E16" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="17" spans="1:4" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
@@ -925,6 +953,9 @@
       <c r="D17" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="E17" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="18" spans="1:4" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
@@ -939,6 +970,9 @@
       <c r="D18" s="4" t="s">
         <v>69</v>
       </c>
+      <c r="E18" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="19" spans="1:4" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="3" t="s">
@@ -953,6 +987,9 @@
       <c r="D19" s="4" t="s">
         <v>72</v>
       </c>
+      <c r="E19" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="20" spans="1:4" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
@@ -966,6 +1003,9 @@
       </c>
       <c r="D20" s="4" t="s">
         <v>75</v>
+      </c>
+      <c r="E20" t="s">
+        <v>76</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update common and create new file
</commit_message>
<xml_diff>
--- a/src/main/resources/excels/BuyLinkTCs.xlsx
+++ b/src/main/resources/excels/BuyLinkTCs.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20361"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67564B56-D131-4DD9-A659-5A223D56147B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C7CA7A6-472A-4A1F-A779-B47DD4E2D259}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -12,7 +12,7 @@
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="78">
   <si>
     <t>TestCase ID</t>
   </si>
@@ -203,9 +203,6 @@
   </si>
   <si>
     <t>Check delete link</t>
-  </si>
-  <si>
-    <t>Result</t>
   </si>
   <si>
     <t>Check navigate to buy link of store that enable guest checkout</t>
@@ -313,14 +310,16 @@
     <t>PASS</t>
   </si>
   <si>
-    <t>FAIL</t>
+    <t>Result ENG</t>
+  </si>
+  <si>
+    <t>Result VIE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -678,7 +677,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E20"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
@@ -686,13 +685,14 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" customWidth="true" width="32.33203125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="65.6640625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="42.0" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="18.0" collapsed="true"/>
+    <col min="2" max="2" width="32.33203125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="65.6640625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="42" customWidth="1" collapsed="1"/>
+    <col min="5" max="5" width="18" customWidth="1" collapsed="1"/>
+    <col min="6" max="6" width="12.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:6" ht="27.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -706,10 +706,13 @@
         <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+        <v>76</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -723,10 +726,10 @@
         <v>7</v>
       </c>
       <c r="E2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -740,10 +743,10 @@
         <v>7</v>
       </c>
       <c r="E3" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
         <v>11</v>
       </c>
@@ -757,10 +760,10 @@
         <v>14</v>
       </c>
       <c r="E4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>15</v>
       </c>
@@ -774,10 +777,10 @@
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>19</v>
       </c>
@@ -791,10 +794,10 @@
         <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="79.8" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="3" t="s">
         <v>22</v>
       </c>
@@ -808,10 +811,10 @@
         <v>25</v>
       </c>
       <c r="E7" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>26</v>
       </c>
@@ -825,10 +828,10 @@
         <v>18</v>
       </c>
       <c r="E8" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>29</v>
       </c>
@@ -842,27 +845,27 @@
         <v>18</v>
       </c>
       <c r="E9" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>32</v>
       </c>
       <c r="B10" s="4" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="D10" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D10" s="4" t="s">
-        <v>54</v>
-      </c>
       <c r="E10" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>35</v>
       </c>
@@ -873,13 +876,13 @@
         <v>34</v>
       </c>
       <c r="D11" s="4" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E11" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>37</v>
       </c>
@@ -887,16 +890,16 @@
         <v>36</v>
       </c>
       <c r="C12" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="D12" s="4" t="s">
-        <v>57</v>
-      </c>
       <c r="E12" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>39</v>
       </c>
@@ -904,16 +907,16 @@
         <v>38</v>
       </c>
       <c r="C13" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="D13" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="4" t="s">
-        <v>59</v>
-      </c>
       <c r="E13" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>41</v>
       </c>
@@ -921,16 +924,16 @@
         <v>40</v>
       </c>
       <c r="C14" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="D14" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="E14" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>43</v>
       </c>
@@ -938,16 +941,16 @@
         <v>42</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>45</v>
       </c>
@@ -955,33 +958,33 @@
         <v>44</v>
       </c>
       <c r="C16" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D16" s="4" t="s">
-        <v>64</v>
-      </c>
       <c r="E16" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B17" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="C17" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D17" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D17" s="4" t="s">
-        <v>67</v>
-      </c>
       <c r="E17" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>49</v>
       </c>
@@ -989,47 +992,47 @@
         <v>46</v>
       </c>
       <c r="C18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="E18" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="E18" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C19" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="3" t="s">
         <v>72</v>
-      </c>
-      <c r="E19" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" ht="53.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="3" t="s">
-        <v>73</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>50</v>
       </c>
       <c r="C20" s="4" t="s">
+        <v>73</v>
+      </c>
+      <c r="D20" s="4" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="4" t="s">
-        <v>75</v>
-      </c>
       <c r="E20" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>

</xml_diff>